<commit_message>
Added TVS diodes on Dyna data lines
Also added parts to BOM
</commit_message>
<xml_diff>
--- a/hardware/v4/Robotic Arm V4 BOM.xlsx
+++ b/hardware/v4/Robotic Arm V4 BOM.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\Robotic-Arm\Hardware\v4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="2430" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="400" yWindow="2440" windowWidth="19820" windowHeight="9400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
   <si>
     <t>Partlist exported from C:/Users/Mike M/Documents/GitHub/Robotic-Arm/hardware/v4/Arm Board V4.sch at 3/9/2015 4:30:44 AM</t>
   </si>
@@ -355,13 +355,34 @@
   </si>
   <si>
     <t>96W2437</t>
+  </si>
+  <si>
+    <t>SMAJ5920</t>
+  </si>
+  <si>
+    <t>DIODE-SCHOTTKY-MBRA140</t>
+  </si>
+  <si>
+    <t>SMA-DIODE</t>
+  </si>
+  <si>
+    <t>D4, D5, D6, D7</t>
+  </si>
+  <si>
+    <t>Schottky diodes in SFE's production catalog</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>51T4985</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -404,6 +425,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -453,6 +480,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,7 +547,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,7 +582,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,26 +794,26 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="4"/>
-    <col min="2" max="2" width="24.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="4"/>
+    <col min="1" max="1" width="14.5" style="4"/>
+    <col min="2" max="2" width="24.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -829,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="7">
         <v>3</v>
       </c>
@@ -856,7 +887,7 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -887,7 +918,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -918,7 +949,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -949,7 +980,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -980,7 +1011,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1011,7 +1042,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -1042,7 +1073,7 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -1073,7 +1104,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1">
       <c r="A11" s="7">
         <v>1</v>
       </c>
@@ -1104,7 +1135,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -1135,7 +1166,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1">
       <c r="A13" s="7">
         <v>1</v>
       </c>
@@ -1166,7 +1197,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1">
       <c r="A14" s="7">
         <v>4</v>
       </c>
@@ -1195,7 +1226,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1">
       <c r="A15" s="7">
         <v>1</v>
       </c>
@@ -1230,7 +1261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1">
       <c r="A16" s="7">
         <v>2</v>
       </c>
@@ -1264,7 +1295,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1284,7 +1315,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -1302,7 +1333,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -1332,7 +1363,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -1360,7 +1391,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1">
       <c r="A21" s="7">
         <v>3</v>
       </c>
@@ -1390,7 +1421,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -1419,7 +1450,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="7">
         <v>1</v>
       </c>
@@ -1458,7 +1489,7 @@
       </c>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="7">
         <v>4</v>
       </c>
@@ -1489,7 +1520,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -1518,7 +1549,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -1547,7 +1578,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -1576,10 +1607,36 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A28" s="13">
+        <v>4</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="11"/>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1596,7 +1653,7 @@
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1613,7 +1670,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1630,7 +1687,7 @@
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1647,7 +1704,7 @@
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1664,7 +1721,7 @@
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1681,7 +1738,7 @@
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1698,7 +1755,7 @@
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="15.75" customHeight="1">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1715,7 +1772,7 @@
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1732,7 +1789,7 @@
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="15.75" customHeight="1">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1749,7 +1806,7 @@
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15.75" customHeight="1">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1766,7 +1823,7 @@
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="15.75" customHeight="1">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1783,7 +1840,7 @@
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="15.75" customHeight="1">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1800,7 +1857,7 @@
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="15.75" customHeight="1">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1817,7 +1874,7 @@
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="15.75" customHeight="1">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1834,7 +1891,7 @@
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="15.75" customHeight="1">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1851,7 +1908,7 @@
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
     </row>
-    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="15.75" customHeight="1">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1868,7 +1925,7 @@
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
-    <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="15.75" customHeight="1">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1885,7 +1942,7 @@
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
-    <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="15.75" customHeight="1">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1902,7 +1959,7 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
     </row>
-    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="15.75" customHeight="1">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1919,7 +1976,7 @@
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
     </row>
-    <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="15.75" customHeight="1">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1936,7 +1993,7 @@
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
     </row>
-    <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="15.75" customHeight="1">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1953,7 +2010,7 @@
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
     </row>
-    <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="15.75" customHeight="1">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1987,6 +2044,11 @@
     <hyperlink ref="J12" r:id="rId13" tooltip="96W2437" display="http://www.newark.com/cornell-dubilier/ave337m06x16t-f/aluminum-electrolytic-capacitor/dp/96W2437"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>